<commit_message>
mudanças de adequação para o trello
</commit_message>
<xml_diff>
--- a/documentação/product_backlog.xlsx
+++ b/documentação/product_backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santd\OneDrive\Documentos\arqsptech\1°semestre\sprint2\PI\Projeto_Individual\documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5372B12-2404-41C4-A647-45AEF20C1F14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21FF0A90-E2AE-4B67-BBC3-42EEAFE0750E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{E62FAEF4-AD96-4A6F-A4C2-09B65FCFF361}"/>
+    <workbookView xWindow="10140" yWindow="0" windowWidth="10455" windowHeight="10905" xr2:uid="{E62FAEF4-AD96-4A6F-A4C2-09B65FCFF361}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -603,33 +603,57 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -655,30 +679,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1022,8 +1022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CF120AB-7321-4195-BFED-264AEC5A03D0}">
   <dimension ref="B2:R55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8:R8"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54:H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,26 +1037,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="O2" s="10" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="O2" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
     </row>
     <row r="3" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
@@ -1065,19 +1065,19 @@
       <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3" t="s">
+      <c r="E3" s="15"/>
+      <c r="F3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3" t="s">
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="3"/>
+      <c r="J3" s="15"/>
       <c r="K3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1087,1203 +1087,1399 @@
       <c r="M3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O3" s="20" t="s">
+      <c r="O3" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="P3" s="11" t="s">
+      <c r="P3" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="13"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="21"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="7" t="s">
+      <c r="E4" s="5"/>
+      <c r="F4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6" t="s">
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6" t="s">
+      <c r="J4" s="5"/>
+      <c r="K4" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="L4" s="6">
+      <c r="L4" s="5">
         <v>13</v>
       </c>
-      <c r="M4" s="6">
+      <c r="M4" s="5">
         <v>1</v>
       </c>
-      <c r="O4" s="20"/>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="16"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="24"/>
     </row>
     <row r="5" spans="2:18" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="O5" s="24" t="s">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="O5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="P5" s="17" t="s">
+      <c r="P5" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="Q5" s="18"/>
-      <c r="R5" s="19"/>
+      <c r="Q5" s="26"/>
+      <c r="R5" s="27"/>
     </row>
     <row r="6" spans="2:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="8" t="s">
+      <c r="E6" s="8"/>
+      <c r="F6" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="2" t="s">
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2" t="s">
+      <c r="J6" s="8"/>
+      <c r="K6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="L6" s="2">
+      <c r="L6" s="8">
         <v>5</v>
       </c>
-      <c r="M6" s="2">
+      <c r="M6" s="8">
         <v>1</v>
       </c>
-      <c r="O6" s="24" t="s">
+      <c r="O6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="P6" s="17" t="s">
+      <c r="P6" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="Q6" s="18"/>
-      <c r="R6" s="19"/>
+      <c r="Q6" s="26"/>
+      <c r="R6" s="27"/>
     </row>
     <row r="7" spans="2:18" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="O7" s="24" t="s">
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="O7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="P7" s="17" t="s">
+      <c r="P7" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="Q7" s="18"/>
-      <c r="R7" s="19"/>
+      <c r="Q7" s="26"/>
+      <c r="R7" s="27"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="8" t="s">
+      <c r="E8" s="8"/>
+      <c r="F8" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="2" t="s">
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2" t="s">
+      <c r="J8" s="8"/>
+      <c r="K8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="L8" s="2">
+      <c r="L8" s="8">
         <v>5</v>
       </c>
-      <c r="M8" s="2">
+      <c r="M8" s="8">
         <v>1</v>
       </c>
-      <c r="O8" s="25" t="s">
+      <c r="O8" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="P8" s="26" t="s">
+      <c r="P8" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="Q8" s="26"/>
-      <c r="R8" s="26"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
     </row>
     <row r="9" spans="2:18" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="O9" s="21" t="s">
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="O9" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="P9" s="21"/>
-      <c r="Q9" s="21"/>
-      <c r="R9" s="21"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="8" t="s">
+      <c r="E10" s="8"/>
+      <c r="F10" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="2" t="s">
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2" t="s">
+      <c r="J10" s="8"/>
+      <c r="K10" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="L10" s="2">
+      <c r="L10" s="8">
         <v>8</v>
       </c>
-      <c r="M10" s="2">
+      <c r="M10" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="8" t="s">
+      <c r="E12" s="8"/>
+      <c r="F12" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="2" t="s">
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2" t="s">
+      <c r="J12" s="8"/>
+      <c r="K12" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="L12" s="2">
+      <c r="L12" s="8">
         <v>5</v>
       </c>
-      <c r="M12" s="2">
+      <c r="M12" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="8" t="s">
+      <c r="E14" s="8"/>
+      <c r="F14" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="2" t="s">
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2" t="s">
+      <c r="J14" s="8"/>
+      <c r="K14" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="L14" s="2">
+      <c r="L14" s="8">
         <v>3</v>
       </c>
-      <c r="M14" s="2">
+      <c r="M14" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="8" t="s">
+      <c r="E16" s="8"/>
+      <c r="F16" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="2" t="s">
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2" t="s">
+      <c r="J16" s="8"/>
+      <c r="K16" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="L16" s="2">
+      <c r="L16" s="8">
         <v>5</v>
       </c>
-      <c r="M16" s="2">
+      <c r="M16" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="8" t="s">
+      <c r="E18" s="8"/>
+      <c r="F18" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="2" t="s">
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2" t="s">
+      <c r="J18" s="8"/>
+      <c r="K18" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="L18" s="2">
+      <c r="L18" s="8">
         <v>3</v>
       </c>
-      <c r="M18" s="2">
+      <c r="M18" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="8" t="s">
+      <c r="E20" s="8"/>
+      <c r="F20" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="2" t="s">
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2" t="s">
+      <c r="J20" s="8"/>
+      <c r="K20" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="L20" s="2">
+      <c r="L20" s="8">
         <v>13</v>
       </c>
-      <c r="M20" s="2">
+      <c r="M20" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="8" t="s">
+      <c r="E22" s="8"/>
+      <c r="F22" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="2" t="s">
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2" t="s">
+      <c r="J22" s="8"/>
+      <c r="K22" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="L22" s="2">
+      <c r="L22" s="8">
         <v>5</v>
       </c>
-      <c r="M22" s="2">
+      <c r="M22" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="8" t="s">
+      <c r="E24" s="8"/>
+      <c r="F24" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="2" t="s">
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2" t="s">
+      <c r="J24" s="8"/>
+      <c r="K24" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="L24" s="2">
+      <c r="L24" s="8">
         <v>5</v>
       </c>
-      <c r="M24" s="2">
+      <c r="M24" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="8"/>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="8" t="s">
+      <c r="E26" s="8"/>
+      <c r="F26" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="2" t="s">
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2" t="s">
+      <c r="J26" s="8"/>
+      <c r="K26" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="L26" s="2">
+      <c r="L26" s="8">
         <v>5</v>
       </c>
-      <c r="M26" s="2">
+      <c r="M26" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="27" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
     </row>
     <row r="28" spans="2:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="D28" s="22" t="s">
+      <c r="D28" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E28" s="23"/>
-      <c r="F28" s="8" t="s">
+      <c r="E28" s="13"/>
+      <c r="F28" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="2" t="s">
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2" t="s">
+      <c r="J28" s="8"/>
+      <c r="K28" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="L28" s="2">
+      <c r="L28" s="8">
         <v>13</v>
       </c>
-      <c r="M28" s="2">
+      <c r="M28" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-      <c r="L29" s="2"/>
-      <c r="M29" s="2"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="8"/>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E30" s="2"/>
-      <c r="F30" s="8" t="s">
+      <c r="E30" s="8"/>
+      <c r="F30" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="2" t="s">
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2" t="s">
+      <c r="J30" s="8"/>
+      <c r="K30" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="L30" s="2">
+      <c r="L30" s="8">
         <v>8</v>
       </c>
-      <c r="M30" s="2">
+      <c r="M30" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="31" spans="2:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="8"/>
+      <c r="M31" s="8"/>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D32" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="E32" s="2"/>
-      <c r="F32" s="8" t="s">
+      <c r="E32" s="8"/>
+      <c r="F32" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="2" t="s">
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2" t="s">
+      <c r="J32" s="8"/>
+      <c r="K32" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="L32" s="2">
+      <c r="L32" s="8">
         <v>5</v>
       </c>
-      <c r="M32" s="2">
+      <c r="M32" s="8">
         <v>3</v>
       </c>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="8"/>
+      <c r="M33" s="8"/>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="E34" s="2"/>
-      <c r="F34" s="8" t="s">
+      <c r="E34" s="8"/>
+      <c r="F34" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="2" t="s">
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2" t="s">
+      <c r="J34" s="8"/>
+      <c r="K34" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="L34" s="2">
+      <c r="L34" s="8">
         <v>5</v>
       </c>
-      <c r="M34" s="2">
+      <c r="M34" s="8">
         <v>3</v>
       </c>
     </row>
     <row r="35" spans="2:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
-      <c r="M35" s="2"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="8"/>
+      <c r="L35" s="8"/>
+      <c r="M35" s="8"/>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D36" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="E36" s="2"/>
-      <c r="F36" s="8" t="s">
+      <c r="E36" s="8"/>
+      <c r="F36" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="G36" s="9"/>
-      <c r="H36" s="9"/>
-      <c r="I36" s="2" t="s">
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2" t="s">
+      <c r="J36" s="8"/>
+      <c r="K36" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="L36" s="2">
+      <c r="L36" s="8">
         <v>5</v>
       </c>
-      <c r="M36" s="2">
+      <c r="M36" s="8">
         <v>3</v>
       </c>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
-      <c r="L37" s="2"/>
-      <c r="M37" s="2"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="8"/>
+      <c r="M37" s="8"/>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D38" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="E38" s="2"/>
-      <c r="F38" s="8" t="s">
+      <c r="E38" s="8"/>
+      <c r="F38" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
-      <c r="I38" s="2" t="s">
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J38" s="2"/>
-      <c r="K38" s="2" t="s">
+      <c r="J38" s="8"/>
+      <c r="K38" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="L38" s="2">
+      <c r="L38" s="8">
         <v>13</v>
       </c>
-      <c r="M38" s="2">
+      <c r="M38" s="8">
         <v>3</v>
       </c>
     </row>
     <row r="39" spans="2:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
-      <c r="K39" s="2"/>
-      <c r="L39" s="2"/>
-      <c r="M39" s="2"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="8"/>
+      <c r="M39" s="8"/>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="D40" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="E40" s="2"/>
-      <c r="F40" s="8" t="s">
+      <c r="E40" s="8"/>
+      <c r="F40" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="G40" s="9"/>
-      <c r="H40" s="9"/>
-      <c r="I40" s="2" t="s">
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2" t="s">
+      <c r="J40" s="8"/>
+      <c r="K40" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="L40" s="2">
+      <c r="L40" s="8">
         <v>13</v>
       </c>
-      <c r="M40" s="2">
+      <c r="M40" s="8">
         <v>3</v>
       </c>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="9"/>
-      <c r="H41" s="9"/>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
-      <c r="L41" s="2"/>
-      <c r="M41" s="2"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8"/>
+      <c r="K41" s="8"/>
+      <c r="L41" s="8"/>
+      <c r="M41" s="8"/>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="D42" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="E42" s="2"/>
-      <c r="F42" s="8" t="s">
+      <c r="E42" s="8"/>
+      <c r="F42" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="G42" s="9"/>
-      <c r="H42" s="9"/>
-      <c r="I42" s="2" t="s">
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J42" s="2"/>
-      <c r="K42" s="2" t="s">
+      <c r="J42" s="8"/>
+      <c r="K42" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="L42" s="2">
+      <c r="L42" s="8">
         <v>8</v>
       </c>
-      <c r="M42" s="2">
+      <c r="M42" s="8">
         <v>3</v>
       </c>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="9"/>
-      <c r="H43" s="9"/>
-      <c r="I43" s="2"/>
-      <c r="J43" s="2"/>
-      <c r="K43" s="2"/>
-      <c r="L43" s="2"/>
-      <c r="M43" s="2"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="8"/>
+      <c r="K43" s="8"/>
+      <c r="L43" s="8"/>
+      <c r="M43" s="8"/>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D44" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="E44" s="2"/>
-      <c r="F44" s="8" t="s">
+      <c r="E44" s="8"/>
+      <c r="F44" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="G44" s="9"/>
-      <c r="H44" s="9"/>
-      <c r="I44" s="2" t="s">
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J44" s="2"/>
-      <c r="K44" s="2" t="s">
+      <c r="J44" s="8"/>
+      <c r="K44" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="L44" s="2">
+      <c r="L44" s="8">
         <v>5</v>
       </c>
-      <c r="M44" s="2">
+      <c r="M44" s="8">
         <v>4</v>
       </c>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="9"/>
-      <c r="H45" s="9"/>
-      <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
-      <c r="K45" s="2"/>
-      <c r="L45" s="2"/>
-      <c r="M45" s="2"/>
+      <c r="B45" s="8"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="8"/>
+      <c r="J45" s="8"/>
+      <c r="K45" s="8"/>
+      <c r="L45" s="8"/>
+      <c r="M45" s="8"/>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D46" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E46" s="2"/>
-      <c r="F46" s="8" t="s">
+      <c r="E46" s="8"/>
+      <c r="F46" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="G46" s="9"/>
-      <c r="H46" s="9"/>
-      <c r="I46" s="2" t="s">
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
+      <c r="I46" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J46" s="2"/>
-      <c r="K46" s="2" t="s">
+      <c r="J46" s="8"/>
+      <c r="K46" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="L46" s="2">
+      <c r="L46" s="8">
         <v>5</v>
       </c>
-      <c r="M46" s="2">
+      <c r="M46" s="8">
         <v>4</v>
       </c>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="9"/>
-      <c r="G47" s="9"/>
-      <c r="H47" s="9"/>
-      <c r="I47" s="2"/>
-      <c r="J47" s="2"/>
-      <c r="K47" s="2"/>
-      <c r="L47" s="2"/>
-      <c r="M47" s="2"/>
+      <c r="B47" s="8"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="8"/>
+      <c r="J47" s="8"/>
+      <c r="K47" s="8"/>
+      <c r="L47" s="8"/>
+      <c r="M47" s="8"/>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C48" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="D48" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="E48" s="2"/>
-      <c r="F48" s="8" t="s">
+      <c r="E48" s="8"/>
+      <c r="F48" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="G48" s="9"/>
-      <c r="H48" s="9"/>
-      <c r="I48" s="2" t="s">
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J48" s="2"/>
-      <c r="K48" s="2" t="s">
+      <c r="J48" s="8"/>
+      <c r="K48" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="L48" s="2">
+      <c r="L48" s="8">
         <v>5</v>
       </c>
-      <c r="M48" s="2">
+      <c r="M48" s="8">
         <v>4</v>
       </c>
     </row>
     <row r="49" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="9"/>
-      <c r="G49" s="9"/>
-      <c r="H49" s="9"/>
-      <c r="I49" s="2"/>
-      <c r="J49" s="2"/>
-      <c r="K49" s="2"/>
-      <c r="L49" s="2"/>
-      <c r="M49" s="2"/>
+      <c r="B49" s="8"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="11"/>
+      <c r="G49" s="11"/>
+      <c r="H49" s="11"/>
+      <c r="I49" s="8"/>
+      <c r="J49" s="8"/>
+      <c r="K49" s="8"/>
+      <c r="L49" s="8"/>
+      <c r="M49" s="8"/>
     </row>
     <row r="50" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B50" s="2" t="s">
+      <c r="B50" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C50" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="D50" s="5" t="s">
+      <c r="D50" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="E50" s="2"/>
-      <c r="F50" s="8" t="s">
+      <c r="E50" s="8"/>
+      <c r="F50" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="G50" s="9"/>
-      <c r="H50" s="9"/>
-      <c r="I50" s="2" t="s">
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J50" s="2"/>
-      <c r="K50" s="2" t="s">
+      <c r="J50" s="8"/>
+      <c r="K50" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="L50" s="2">
+      <c r="L50" s="8">
         <v>13</v>
       </c>
-      <c r="M50" s="2">
+      <c r="M50" s="8">
         <v>4</v>
       </c>
     </row>
     <row r="51" spans="2:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
-      <c r="F51" s="9"/>
-      <c r="G51" s="9"/>
-      <c r="H51" s="9"/>
-      <c r="I51" s="2"/>
-      <c r="J51" s="2"/>
-      <c r="K51" s="2"/>
-      <c r="L51" s="2"/>
-      <c r="M51" s="2"/>
+      <c r="B51" s="8"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="8"/>
+      <c r="F51" s="11"/>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="8"/>
+      <c r="J51" s="8"/>
+      <c r="K51" s="8"/>
+      <c r="L51" s="8"/>
+      <c r="M51" s="8"/>
     </row>
     <row r="52" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B52" s="6" t="s">
+      <c r="B52" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C52" s="6" t="s">
+      <c r="C52" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="D52" s="6" t="s">
+      <c r="D52" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="E52" s="6"/>
-      <c r="F52" s="7" t="s">
+      <c r="E52" s="5"/>
+      <c r="F52" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="G52" s="27"/>
-      <c r="H52" s="27"/>
-      <c r="I52" s="6" t="s">
+      <c r="G52" s="7"/>
+      <c r="H52" s="7"/>
+      <c r="I52" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="J52" s="6"/>
-      <c r="K52" s="6" t="s">
+      <c r="J52" s="5"/>
+      <c r="K52" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="L52" s="6">
+      <c r="L52" s="5">
         <v>8</v>
       </c>
-      <c r="M52" s="6">
+      <c r="M52" s="5">
         <v>4</v>
       </c>
     </row>
     <row r="53" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B53" s="6"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="6"/>
-      <c r="E53" s="6"/>
-      <c r="F53" s="27"/>
-      <c r="G53" s="27"/>
-      <c r="H53" s="27"/>
-      <c r="I53" s="6"/>
-      <c r="J53" s="6"/>
-      <c r="K53" s="6"/>
-      <c r="L53" s="6"/>
-      <c r="M53" s="6"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="7"/>
+      <c r="H53" s="7"/>
+      <c r="I53" s="5"/>
+      <c r="J53" s="5"/>
+      <c r="K53" s="5"/>
+      <c r="L53" s="5"/>
+      <c r="M53" s="5"/>
     </row>
     <row r="54" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B54" s="6" t="s">
+      <c r="B54" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C54" s="6" t="s">
+      <c r="C54" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D54" s="6" t="s">
+      <c r="D54" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="E54" s="6"/>
-      <c r="F54" s="7" t="s">
+      <c r="E54" s="5"/>
+      <c r="F54" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="G54" s="27"/>
-      <c r="H54" s="27"/>
-      <c r="I54" s="6" t="s">
+      <c r="G54" s="7"/>
+      <c r="H54" s="7"/>
+      <c r="I54" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="J54" s="6"/>
-      <c r="K54" s="6" t="s">
+      <c r="J54" s="5"/>
+      <c r="K54" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="L54" s="6">
+      <c r="L54" s="5">
         <v>13</v>
       </c>
-      <c r="M54" s="6">
+      <c r="M54" s="5">
         <v>4</v>
       </c>
     </row>
     <row r="55" spans="2:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="6"/>
-      <c r="C55" s="6"/>
-      <c r="D55" s="6"/>
-      <c r="E55" s="6"/>
-      <c r="F55" s="27"/>
-      <c r="G55" s="27"/>
-      <c r="H55" s="27"/>
-      <c r="I55" s="6"/>
-      <c r="J55" s="6"/>
-      <c r="K55" s="6"/>
-      <c r="L55" s="6"/>
-      <c r="M55" s="6"/>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="7"/>
+      <c r="H55" s="7"/>
+      <c r="I55" s="5"/>
+      <c r="J55" s="5"/>
+      <c r="K55" s="5"/>
+      <c r="L55" s="5"/>
+      <c r="M55" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="220">
+    <mergeCell ref="L20:L21"/>
+    <mergeCell ref="M20:M21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:E21"/>
+    <mergeCell ref="F20:H21"/>
+    <mergeCell ref="I20:J21"/>
+    <mergeCell ref="K20:K21"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:E19"/>
+    <mergeCell ref="F18:H19"/>
+    <mergeCell ref="I18:J19"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:E17"/>
+    <mergeCell ref="F16:H17"/>
+    <mergeCell ref="I16:J17"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="M12:M13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:E15"/>
+    <mergeCell ref="F14:H15"/>
+    <mergeCell ref="I14:J15"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:E13"/>
+    <mergeCell ref="F12:H13"/>
+    <mergeCell ref="I12:J13"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="P7:R7"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:E7"/>
+    <mergeCell ref="F6:H7"/>
+    <mergeCell ref="I6:J7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:E5"/>
+    <mergeCell ref="F4:H5"/>
+    <mergeCell ref="I4:J5"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="P3:R4"/>
+    <mergeCell ref="P5:R5"/>
+    <mergeCell ref="P6:R6"/>
+    <mergeCell ref="O9:R9"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:E23"/>
+    <mergeCell ref="F22:H23"/>
+    <mergeCell ref="I22:J23"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:E11"/>
+    <mergeCell ref="F10:H11"/>
+    <mergeCell ref="I10:J11"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="M10:M11"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:E9"/>
+    <mergeCell ref="F8:H9"/>
+    <mergeCell ref="I8:J9"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="L24:L25"/>
+    <mergeCell ref="M24:M25"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:E27"/>
+    <mergeCell ref="F26:H27"/>
+    <mergeCell ref="I26:J27"/>
+    <mergeCell ref="K26:K27"/>
+    <mergeCell ref="L26:L27"/>
+    <mergeCell ref="M26:M27"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:E25"/>
+    <mergeCell ref="F24:H25"/>
+    <mergeCell ref="I24:J25"/>
+    <mergeCell ref="K28:K29"/>
+    <mergeCell ref="L28:L29"/>
+    <mergeCell ref="M28:M29"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:E31"/>
+    <mergeCell ref="F30:H31"/>
+    <mergeCell ref="I30:J31"/>
+    <mergeCell ref="K30:K31"/>
+    <mergeCell ref="L30:L31"/>
+    <mergeCell ref="M30:M31"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:E29"/>
+    <mergeCell ref="F28:H29"/>
+    <mergeCell ref="I28:J29"/>
+    <mergeCell ref="K32:K33"/>
+    <mergeCell ref="L32:L33"/>
+    <mergeCell ref="M32:M33"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D34:E35"/>
+    <mergeCell ref="F34:H35"/>
+    <mergeCell ref="I34:J35"/>
+    <mergeCell ref="K34:K35"/>
+    <mergeCell ref="L34:L35"/>
+    <mergeCell ref="M34:M35"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:E33"/>
+    <mergeCell ref="F32:H33"/>
+    <mergeCell ref="I32:J33"/>
+    <mergeCell ref="K36:K37"/>
+    <mergeCell ref="L36:L37"/>
+    <mergeCell ref="M36:M37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="D38:E39"/>
+    <mergeCell ref="F38:H39"/>
+    <mergeCell ref="I38:J39"/>
+    <mergeCell ref="K38:K39"/>
+    <mergeCell ref="L38:L39"/>
+    <mergeCell ref="M38:M39"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="D36:E37"/>
+    <mergeCell ref="F36:H37"/>
+    <mergeCell ref="I36:J37"/>
+    <mergeCell ref="K40:K41"/>
+    <mergeCell ref="L40:L41"/>
+    <mergeCell ref="M40:M41"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:E43"/>
+    <mergeCell ref="F42:H43"/>
+    <mergeCell ref="I42:J43"/>
+    <mergeCell ref="K42:K43"/>
+    <mergeCell ref="L42:L43"/>
+    <mergeCell ref="M42:M43"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="D40:E41"/>
+    <mergeCell ref="F40:H41"/>
+    <mergeCell ref="I40:J41"/>
+    <mergeCell ref="K44:K45"/>
+    <mergeCell ref="L44:L45"/>
+    <mergeCell ref="M44:M45"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D46:E47"/>
+    <mergeCell ref="F46:H47"/>
+    <mergeCell ref="I46:J47"/>
+    <mergeCell ref="K46:K47"/>
+    <mergeCell ref="L46:L47"/>
+    <mergeCell ref="M46:M47"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:E45"/>
+    <mergeCell ref="F44:H45"/>
+    <mergeCell ref="I44:J45"/>
+    <mergeCell ref="I50:J51"/>
+    <mergeCell ref="K50:K51"/>
+    <mergeCell ref="L50:L51"/>
+    <mergeCell ref="M50:M51"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="D48:E49"/>
+    <mergeCell ref="F48:H49"/>
+    <mergeCell ref="I48:J49"/>
     <mergeCell ref="P8:R8"/>
     <mergeCell ref="K52:K53"/>
     <mergeCell ref="L52:L53"/>
@@ -2308,202 +2504,6 @@
     <mergeCell ref="C50:C51"/>
     <mergeCell ref="D50:E51"/>
     <mergeCell ref="F50:H51"/>
-    <mergeCell ref="I50:J51"/>
-    <mergeCell ref="K50:K51"/>
-    <mergeCell ref="L50:L51"/>
-    <mergeCell ref="M50:M51"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:E49"/>
-    <mergeCell ref="F48:H49"/>
-    <mergeCell ref="I48:J49"/>
-    <mergeCell ref="K44:K45"/>
-    <mergeCell ref="L44:L45"/>
-    <mergeCell ref="M44:M45"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="D46:E47"/>
-    <mergeCell ref="F46:H47"/>
-    <mergeCell ref="I46:J47"/>
-    <mergeCell ref="K46:K47"/>
-    <mergeCell ref="L46:L47"/>
-    <mergeCell ref="M46:M47"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D44:E45"/>
-    <mergeCell ref="F44:H45"/>
-    <mergeCell ref="I44:J45"/>
-    <mergeCell ref="K40:K41"/>
-    <mergeCell ref="L40:L41"/>
-    <mergeCell ref="M40:M41"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D42:E43"/>
-    <mergeCell ref="F42:H43"/>
-    <mergeCell ref="I42:J43"/>
-    <mergeCell ref="K42:K43"/>
-    <mergeCell ref="L42:L43"/>
-    <mergeCell ref="M42:M43"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="D40:E41"/>
-    <mergeCell ref="F40:H41"/>
-    <mergeCell ref="I40:J41"/>
-    <mergeCell ref="K36:K37"/>
-    <mergeCell ref="L36:L37"/>
-    <mergeCell ref="M36:M37"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="D38:E39"/>
-    <mergeCell ref="F38:H39"/>
-    <mergeCell ref="I38:J39"/>
-    <mergeCell ref="K38:K39"/>
-    <mergeCell ref="L38:L39"/>
-    <mergeCell ref="M38:M39"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="D36:E37"/>
-    <mergeCell ref="F36:H37"/>
-    <mergeCell ref="I36:J37"/>
-    <mergeCell ref="K32:K33"/>
-    <mergeCell ref="L32:L33"/>
-    <mergeCell ref="M32:M33"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="D34:E35"/>
-    <mergeCell ref="F34:H35"/>
-    <mergeCell ref="I34:J35"/>
-    <mergeCell ref="K34:K35"/>
-    <mergeCell ref="L34:L35"/>
-    <mergeCell ref="M34:M35"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:E33"/>
-    <mergeCell ref="F32:H33"/>
-    <mergeCell ref="I32:J33"/>
-    <mergeCell ref="K28:K29"/>
-    <mergeCell ref="L28:L29"/>
-    <mergeCell ref="M28:M29"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:E31"/>
-    <mergeCell ref="F30:H31"/>
-    <mergeCell ref="I30:J31"/>
-    <mergeCell ref="K30:K31"/>
-    <mergeCell ref="L30:L31"/>
-    <mergeCell ref="M30:M31"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:E29"/>
-    <mergeCell ref="F28:H29"/>
-    <mergeCell ref="I28:J29"/>
-    <mergeCell ref="K24:K25"/>
-    <mergeCell ref="L24:L25"/>
-    <mergeCell ref="M24:M25"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:E27"/>
-    <mergeCell ref="F26:H27"/>
-    <mergeCell ref="I26:J27"/>
-    <mergeCell ref="K26:K27"/>
-    <mergeCell ref="L26:L27"/>
-    <mergeCell ref="M26:M27"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:E25"/>
-    <mergeCell ref="F24:H25"/>
-    <mergeCell ref="I24:J25"/>
-    <mergeCell ref="O9:R9"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:E23"/>
-    <mergeCell ref="F22:H23"/>
-    <mergeCell ref="I22:J23"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="M22:M23"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="B2:M2"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="O3:O4"/>
-    <mergeCell ref="P3:R4"/>
-    <mergeCell ref="P5:R5"/>
-    <mergeCell ref="P6:R6"/>
-    <mergeCell ref="P7:R7"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:E7"/>
-    <mergeCell ref="F6:H7"/>
-    <mergeCell ref="I6:J7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:E5"/>
-    <mergeCell ref="F4:H5"/>
-    <mergeCell ref="I4:J5"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:E11"/>
-    <mergeCell ref="F10:H11"/>
-    <mergeCell ref="I10:J11"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="L10:L11"/>
-    <mergeCell ref="M10:M11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:E9"/>
-    <mergeCell ref="F8:H9"/>
-    <mergeCell ref="I8:J9"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="M12:M13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:E15"/>
-    <mergeCell ref="F14:H15"/>
-    <mergeCell ref="I14:J15"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:E13"/>
-    <mergeCell ref="F12:H13"/>
-    <mergeCell ref="I12:J13"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="L16:L17"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:E19"/>
-    <mergeCell ref="F18:H19"/>
-    <mergeCell ref="I18:J19"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="L18:L19"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:E17"/>
-    <mergeCell ref="F16:H17"/>
-    <mergeCell ref="I16:J17"/>
-    <mergeCell ref="K16:K17"/>
-    <mergeCell ref="L20:L21"/>
-    <mergeCell ref="M20:M21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:E21"/>
-    <mergeCell ref="F20:H21"/>
-    <mergeCell ref="I20:J21"/>
-    <mergeCell ref="K20:K21"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>